<commit_message>
add validate missing data checking mechanism
</commit_message>
<xml_diff>
--- a/Wernau_Output.xlsx
+++ b/Wernau_Output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2881"/>
+  <dimension ref="A1:C2977"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -49410,6 +49410,1638 @@
         </is>
       </c>
     </row>
+    <row r="2882">
+      <c r="A2882" t="inlineStr">
+        <is>
+          <t>31.01.2025 00:15</t>
+        </is>
+      </c>
+      <c r="B2882" t="inlineStr">
+        <is>
+          <t>2,12</t>
+        </is>
+      </c>
+      <c r="C2882" t="inlineStr">
+        <is>
+          <t>39,36</t>
+        </is>
+      </c>
+    </row>
+    <row r="2883">
+      <c r="A2883" t="inlineStr">
+        <is>
+          <t>31.01.2025 00:30</t>
+        </is>
+      </c>
+      <c r="B2883" t="inlineStr">
+        <is>
+          <t>10,36</t>
+        </is>
+      </c>
+      <c r="C2883" t="inlineStr">
+        <is>
+          <t>7,12</t>
+        </is>
+      </c>
+    </row>
+    <row r="2884">
+      <c r="A2884" t="inlineStr">
+        <is>
+          <t>31.01.2025 00:45</t>
+        </is>
+      </c>
+      <c r="B2884" t="inlineStr">
+        <is>
+          <t>4,44</t>
+        </is>
+      </c>
+      <c r="C2884" t="inlineStr">
+        <is>
+          <t>41,56</t>
+        </is>
+      </c>
+    </row>
+    <row r="2885">
+      <c r="A2885" t="inlineStr">
+        <is>
+          <t>31.01.2025 01:00</t>
+        </is>
+      </c>
+      <c r="B2885" t="inlineStr">
+        <is>
+          <t>9,12</t>
+        </is>
+      </c>
+      <c r="C2885" t="inlineStr">
+        <is>
+          <t>7,84</t>
+        </is>
+      </c>
+    </row>
+    <row r="2886">
+      <c r="A2886" t="inlineStr">
+        <is>
+          <t>31.01.2025 01:15</t>
+        </is>
+      </c>
+      <c r="B2886" t="inlineStr">
+        <is>
+          <t>16,56</t>
+        </is>
+      </c>
+      <c r="C2886" t="inlineStr">
+        <is>
+          <t>53,76</t>
+        </is>
+      </c>
+    </row>
+    <row r="2887">
+      <c r="A2887" t="inlineStr">
+        <is>
+          <t>31.01.2025 01:30</t>
+        </is>
+      </c>
+      <c r="B2887" t="inlineStr">
+        <is>
+          <t>12,68</t>
+        </is>
+      </c>
+      <c r="C2887" t="inlineStr">
+        <is>
+          <t>13,52</t>
+        </is>
+      </c>
+    </row>
+    <row r="2888">
+      <c r="A2888" t="inlineStr">
+        <is>
+          <t>31.01.2025 01:45</t>
+        </is>
+      </c>
+      <c r="B2888" t="inlineStr">
+        <is>
+          <t>9,6</t>
+        </is>
+      </c>
+      <c r="C2888" t="inlineStr">
+        <is>
+          <t>13,48</t>
+        </is>
+      </c>
+    </row>
+    <row r="2889">
+      <c r="A2889" t="inlineStr">
+        <is>
+          <t>31.01.2025 02:00</t>
+        </is>
+      </c>
+      <c r="B2889" t="inlineStr">
+        <is>
+          <t>174,88</t>
+        </is>
+      </c>
+      <c r="C2889" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2890">
+      <c r="A2890" t="inlineStr">
+        <is>
+          <t>31.01.2025 02:15</t>
+        </is>
+      </c>
+      <c r="B2890" t="inlineStr">
+        <is>
+          <t>14,04</t>
+        </is>
+      </c>
+      <c r="C2890" t="inlineStr">
+        <is>
+          <t>18,48</t>
+        </is>
+      </c>
+    </row>
+    <row r="2891">
+      <c r="A2891" t="inlineStr">
+        <is>
+          <t>31.01.2025 02:30</t>
+        </is>
+      </c>
+      <c r="B2891" t="inlineStr">
+        <is>
+          <t>3,8</t>
+        </is>
+      </c>
+      <c r="C2891" t="inlineStr">
+        <is>
+          <t>28,56</t>
+        </is>
+      </c>
+    </row>
+    <row r="2892">
+      <c r="A2892" t="inlineStr">
+        <is>
+          <t>31.01.2025 02:45</t>
+        </is>
+      </c>
+      <c r="B2892" t="inlineStr">
+        <is>
+          <t>11,44</t>
+        </is>
+      </c>
+      <c r="C2892" t="inlineStr">
+        <is>
+          <t>36,48</t>
+        </is>
+      </c>
+    </row>
+    <row r="2893">
+      <c r="A2893" t="inlineStr">
+        <is>
+          <t>31.01.2025 03:00</t>
+        </is>
+      </c>
+      <c r="B2893" t="inlineStr">
+        <is>
+          <t>6,32</t>
+        </is>
+      </c>
+      <c r="C2893" t="inlineStr">
+        <is>
+          <t>5,12</t>
+        </is>
+      </c>
+    </row>
+    <row r="2894">
+      <c r="A2894" t="inlineStr">
+        <is>
+          <t>31.01.2025 03:15</t>
+        </is>
+      </c>
+      <c r="B2894" t="inlineStr">
+        <is>
+          <t>0,24</t>
+        </is>
+      </c>
+      <c r="C2894" t="inlineStr">
+        <is>
+          <t>51,72</t>
+        </is>
+      </c>
+    </row>
+    <row r="2895">
+      <c r="A2895" t="inlineStr">
+        <is>
+          <t>31.01.2025 03:30</t>
+        </is>
+      </c>
+      <c r="B2895" t="inlineStr">
+        <is>
+          <t>3,64</t>
+        </is>
+      </c>
+      <c r="C2895" t="inlineStr">
+        <is>
+          <t>19,88</t>
+        </is>
+      </c>
+    </row>
+    <row r="2896">
+      <c r="A2896" t="inlineStr">
+        <is>
+          <t>31.01.2025 03:45</t>
+        </is>
+      </c>
+      <c r="B2896" t="inlineStr">
+        <is>
+          <t>0,12</t>
+        </is>
+      </c>
+      <c r="C2896" t="inlineStr">
+        <is>
+          <t>50,92</t>
+        </is>
+      </c>
+    </row>
+    <row r="2897">
+      <c r="A2897" t="inlineStr">
+        <is>
+          <t>31.01.2025 04:00</t>
+        </is>
+      </c>
+      <c r="B2897" t="inlineStr">
+        <is>
+          <t>2,68</t>
+        </is>
+      </c>
+      <c r="C2897" t="inlineStr">
+        <is>
+          <t>19,32</t>
+        </is>
+      </c>
+    </row>
+    <row r="2898">
+      <c r="A2898" t="inlineStr">
+        <is>
+          <t>31.01.2025 04:15</t>
+        </is>
+      </c>
+      <c r="B2898" t="inlineStr">
+        <is>
+          <t>146,4</t>
+        </is>
+      </c>
+      <c r="C2898" t="inlineStr">
+        <is>
+          <t>0,24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2899">
+      <c r="A2899" t="inlineStr">
+        <is>
+          <t>31.01.2025 04:30</t>
+        </is>
+      </c>
+      <c r="B2899" t="inlineStr">
+        <is>
+          <t>8,88</t>
+        </is>
+      </c>
+      <c r="C2899" t="inlineStr">
+        <is>
+          <t>15,64</t>
+        </is>
+      </c>
+    </row>
+    <row r="2900">
+      <c r="A2900" t="inlineStr">
+        <is>
+          <t>31.01.2025 04:45</t>
+        </is>
+      </c>
+      <c r="B2900" t="inlineStr">
+        <is>
+          <t>0,32</t>
+        </is>
+      </c>
+      <c r="C2900" t="inlineStr">
+        <is>
+          <t>37,32</t>
+        </is>
+      </c>
+    </row>
+    <row r="2901">
+      <c r="A2901" t="inlineStr">
+        <is>
+          <t>31.01.2025 05:00</t>
+        </is>
+      </c>
+      <c r="B2901" t="inlineStr">
+        <is>
+          <t>3,56</t>
+        </is>
+      </c>
+      <c r="C2901" t="inlineStr">
+        <is>
+          <t>24,92</t>
+        </is>
+      </c>
+    </row>
+    <row r="2902">
+      <c r="A2902" t="inlineStr">
+        <is>
+          <t>31.01.2025 05:15</t>
+        </is>
+      </c>
+      <c r="B2902" t="inlineStr">
+        <is>
+          <t>29,84</t>
+        </is>
+      </c>
+      <c r="C2902" t="inlineStr">
+        <is>
+          <t>30,12</t>
+        </is>
+      </c>
+    </row>
+    <row r="2903">
+      <c r="A2903" t="inlineStr">
+        <is>
+          <t>31.01.2025 05:30</t>
+        </is>
+      </c>
+      <c r="B2903" t="inlineStr">
+        <is>
+          <t>124,48</t>
+        </is>
+      </c>
+      <c r="C2903" t="inlineStr">
+        <is>
+          <t>0,16</t>
+        </is>
+      </c>
+    </row>
+    <row r="2904">
+      <c r="A2904" t="inlineStr">
+        <is>
+          <t>31.01.2025 05:45</t>
+        </is>
+      </c>
+      <c r="B2904" t="inlineStr">
+        <is>
+          <t>18,48</t>
+        </is>
+      </c>
+      <c r="C2904" t="inlineStr">
+        <is>
+          <t>22,04</t>
+        </is>
+      </c>
+    </row>
+    <row r="2905">
+      <c r="A2905" t="inlineStr">
+        <is>
+          <t>31.01.2025 06:00</t>
+        </is>
+      </c>
+      <c r="B2905" t="inlineStr">
+        <is>
+          <t>18,28</t>
+        </is>
+      </c>
+      <c r="C2905" t="inlineStr">
+        <is>
+          <t>24,28</t>
+        </is>
+      </c>
+    </row>
+    <row r="2906">
+      <c r="A2906" t="inlineStr">
+        <is>
+          <t>31.01.2025 06:15</t>
+        </is>
+      </c>
+      <c r="B2906" t="inlineStr">
+        <is>
+          <t>9,24</t>
+        </is>
+      </c>
+      <c r="C2906" t="inlineStr">
+        <is>
+          <t>83,08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2907">
+      <c r="A2907" t="inlineStr">
+        <is>
+          <t>31.01.2025 06:30</t>
+        </is>
+      </c>
+      <c r="B2907" t="inlineStr">
+        <is>
+          <t>0,92</t>
+        </is>
+      </c>
+      <c r="C2907" t="inlineStr">
+        <is>
+          <t>38,56</t>
+        </is>
+      </c>
+    </row>
+    <row r="2908">
+      <c r="A2908" t="inlineStr">
+        <is>
+          <t>31.01.2025 06:45</t>
+        </is>
+      </c>
+      <c r="B2908" t="inlineStr">
+        <is>
+          <t>0,08</t>
+        </is>
+      </c>
+      <c r="C2908" t="inlineStr">
+        <is>
+          <t>52,92</t>
+        </is>
+      </c>
+    </row>
+    <row r="2909">
+      <c r="A2909" t="inlineStr">
+        <is>
+          <t>31.01.2025 07:00</t>
+        </is>
+      </c>
+      <c r="B2909" t="inlineStr">
+        <is>
+          <t>2,92</t>
+        </is>
+      </c>
+      <c r="C2909" t="inlineStr">
+        <is>
+          <t>69,6</t>
+        </is>
+      </c>
+    </row>
+    <row r="2910">
+      <c r="A2910" t="inlineStr">
+        <is>
+          <t>31.01.2025 07:15</t>
+        </is>
+      </c>
+      <c r="B2910" t="inlineStr">
+        <is>
+          <t>172,2</t>
+        </is>
+      </c>
+      <c r="C2910" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2911">
+      <c r="A2911" t="inlineStr">
+        <is>
+          <t>31.01.2025 07:30</t>
+        </is>
+      </c>
+      <c r="B2911" t="inlineStr">
+        <is>
+          <t>4,4</t>
+        </is>
+      </c>
+      <c r="C2911" t="inlineStr">
+        <is>
+          <t>46,76</t>
+        </is>
+      </c>
+    </row>
+    <row r="2912">
+      <c r="A2912" t="inlineStr">
+        <is>
+          <t>31.01.2025 07:45</t>
+        </is>
+      </c>
+      <c r="B2912" t="inlineStr">
+        <is>
+          <t>136,32</t>
+        </is>
+      </c>
+      <c r="C2912" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2913">
+      <c r="A2913" t="inlineStr">
+        <is>
+          <t>31.01.2025 08:00</t>
+        </is>
+      </c>
+      <c r="B2913" t="inlineStr">
+        <is>
+          <t>11,88</t>
+        </is>
+      </c>
+      <c r="C2913" t="inlineStr">
+        <is>
+          <t>25,56</t>
+        </is>
+      </c>
+    </row>
+    <row r="2914">
+      <c r="A2914" t="inlineStr">
+        <is>
+          <t>31.01.2025 08:15</t>
+        </is>
+      </c>
+      <c r="B2914" t="inlineStr">
+        <is>
+          <t>2,04</t>
+        </is>
+      </c>
+      <c r="C2914" t="inlineStr">
+        <is>
+          <t>41,48</t>
+        </is>
+      </c>
+    </row>
+    <row r="2915">
+      <c r="A2915" t="inlineStr">
+        <is>
+          <t>31.01.2025 08:30</t>
+        </is>
+      </c>
+      <c r="B2915" t="inlineStr">
+        <is>
+          <t>8,24</t>
+        </is>
+      </c>
+      <c r="C2915" t="inlineStr">
+        <is>
+          <t>22,2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2916">
+      <c r="A2916" t="inlineStr">
+        <is>
+          <t>31.01.2025 08:45</t>
+        </is>
+      </c>
+      <c r="B2916" t="inlineStr">
+        <is>
+          <t>6,36</t>
+        </is>
+      </c>
+      <c r="C2916" t="inlineStr">
+        <is>
+          <t>15,84</t>
+        </is>
+      </c>
+    </row>
+    <row r="2917">
+      <c r="A2917" t="inlineStr">
+        <is>
+          <t>31.01.2025 09:00</t>
+        </is>
+      </c>
+      <c r="B2917" t="inlineStr">
+        <is>
+          <t>18,08</t>
+        </is>
+      </c>
+      <c r="C2917" t="inlineStr">
+        <is>
+          <t>14,68</t>
+        </is>
+      </c>
+    </row>
+    <row r="2918">
+      <c r="A2918" t="inlineStr">
+        <is>
+          <t>31.01.2025 09:15</t>
+        </is>
+      </c>
+      <c r="B2918" t="inlineStr">
+        <is>
+          <t>118,04</t>
+        </is>
+      </c>
+      <c r="C2918" t="inlineStr">
+        <is>
+          <t>7,84</t>
+        </is>
+      </c>
+    </row>
+    <row r="2919">
+      <c r="A2919" t="inlineStr">
+        <is>
+          <t>31.01.2025 09:30</t>
+        </is>
+      </c>
+      <c r="B2919" t="inlineStr">
+        <is>
+          <t>22,36</t>
+        </is>
+      </c>
+      <c r="C2919" t="inlineStr">
+        <is>
+          <t>4,36</t>
+        </is>
+      </c>
+    </row>
+    <row r="2920">
+      <c r="A2920" t="inlineStr">
+        <is>
+          <t>31.01.2025 09:45</t>
+        </is>
+      </c>
+      <c r="B2920" t="inlineStr">
+        <is>
+          <t>40,72</t>
+        </is>
+      </c>
+      <c r="C2920" t="inlineStr">
+        <is>
+          <t>22,64</t>
+        </is>
+      </c>
+    </row>
+    <row r="2921">
+      <c r="A2921" t="inlineStr">
+        <is>
+          <t>31.01.2025 10:00</t>
+        </is>
+      </c>
+      <c r="B2921" t="inlineStr">
+        <is>
+          <t>20,2</t>
+        </is>
+      </c>
+      <c r="C2921" t="inlineStr">
+        <is>
+          <t>17,52</t>
+        </is>
+      </c>
+    </row>
+    <row r="2922">
+      <c r="A2922" t="inlineStr">
+        <is>
+          <t>31.01.2025 10:15</t>
+        </is>
+      </c>
+      <c r="B2922" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C2922" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+    </row>
+    <row r="2923">
+      <c r="A2923" t="inlineStr">
+        <is>
+          <t>31.01.2025 10:30</t>
+        </is>
+      </c>
+      <c r="B2923" t="inlineStr">
+        <is>
+          <t>30,56</t>
+        </is>
+      </c>
+      <c r="C2923" t="inlineStr">
+        <is>
+          <t>11,92</t>
+        </is>
+      </c>
+    </row>
+    <row r="2924">
+      <c r="A2924" t="inlineStr">
+        <is>
+          <t>31.01.2025 10:45</t>
+        </is>
+      </c>
+      <c r="B2924" t="inlineStr">
+        <is>
+          <t>9,68</t>
+        </is>
+      </c>
+      <c r="C2924" t="inlineStr">
+        <is>
+          <t>48,72</t>
+        </is>
+      </c>
+    </row>
+    <row r="2925">
+      <c r="A2925" t="inlineStr">
+        <is>
+          <t>31.01.2025 11:00</t>
+        </is>
+      </c>
+      <c r="B2925" t="inlineStr">
+        <is>
+          <t>223</t>
+        </is>
+      </c>
+      <c r="C2925" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2926">
+      <c r="A2926" t="inlineStr">
+        <is>
+          <t>31.01.2025 11:15</t>
+        </is>
+      </c>
+      <c r="B2926" t="inlineStr">
+        <is>
+          <t>12,36</t>
+        </is>
+      </c>
+      <c r="C2926" t="inlineStr">
+        <is>
+          <t>49,72</t>
+        </is>
+      </c>
+    </row>
+    <row r="2927">
+      <c r="A2927" t="inlineStr">
+        <is>
+          <t>31.01.2025 11:30</t>
+        </is>
+      </c>
+      <c r="B2927" t="inlineStr">
+        <is>
+          <t>16,96</t>
+        </is>
+      </c>
+      <c r="C2927" t="inlineStr">
+        <is>
+          <t>17,68</t>
+        </is>
+      </c>
+    </row>
+    <row r="2928">
+      <c r="A2928" t="inlineStr">
+        <is>
+          <t>31.01.2025 11:45</t>
+        </is>
+      </c>
+      <c r="B2928" t="inlineStr">
+        <is>
+          <t>37,8</t>
+        </is>
+      </c>
+      <c r="C2928" t="inlineStr">
+        <is>
+          <t>13,6</t>
+        </is>
+      </c>
+    </row>
+    <row r="2929">
+      <c r="A2929" t="inlineStr">
+        <is>
+          <t>31.01.2025 12:00</t>
+        </is>
+      </c>
+      <c r="B2929" t="inlineStr">
+        <is>
+          <t>38,64</t>
+        </is>
+      </c>
+      <c r="C2929" t="inlineStr">
+        <is>
+          <t>5,2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2930">
+      <c r="A2930" t="inlineStr">
+        <is>
+          <t>31.01.2025 12:15</t>
+        </is>
+      </c>
+      <c r="B2930" t="inlineStr">
+        <is>
+          <t>10,96</t>
+        </is>
+      </c>
+      <c r="C2930" t="inlineStr">
+        <is>
+          <t>27,12</t>
+        </is>
+      </c>
+    </row>
+    <row r="2931">
+      <c r="A2931" t="inlineStr">
+        <is>
+          <t>31.01.2025 12:30</t>
+        </is>
+      </c>
+      <c r="B2931" t="inlineStr">
+        <is>
+          <t>32,84</t>
+        </is>
+      </c>
+      <c r="C2931" t="inlineStr">
+        <is>
+          <t>2,44</t>
+        </is>
+      </c>
+    </row>
+    <row r="2932">
+      <c r="A2932" t="inlineStr">
+        <is>
+          <t>31.01.2025 12:45</t>
+        </is>
+      </c>
+      <c r="B2932" t="inlineStr">
+        <is>
+          <t>11,08</t>
+        </is>
+      </c>
+      <c r="C2932" t="inlineStr">
+        <is>
+          <t>29,32</t>
+        </is>
+      </c>
+    </row>
+    <row r="2933">
+      <c r="A2933" t="inlineStr">
+        <is>
+          <t>31.01.2025 13:00</t>
+        </is>
+      </c>
+      <c r="B2933" t="inlineStr">
+        <is>
+          <t>43,88</t>
+        </is>
+      </c>
+      <c r="C2933" t="inlineStr">
+        <is>
+          <t>5,96</t>
+        </is>
+      </c>
+    </row>
+    <row r="2934">
+      <c r="A2934" t="inlineStr">
+        <is>
+          <t>31.01.2025 13:15</t>
+        </is>
+      </c>
+      <c r="B2934" t="inlineStr">
+        <is>
+          <t>7,24</t>
+        </is>
+      </c>
+      <c r="C2934" t="inlineStr">
+        <is>
+          <t>11,4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2935">
+      <c r="A2935" t="inlineStr">
+        <is>
+          <t>31.01.2025 13:30</t>
+        </is>
+      </c>
+      <c r="B2935" t="inlineStr">
+        <is>
+          <t>2,32</t>
+        </is>
+      </c>
+      <c r="C2935" t="inlineStr">
+        <is>
+          <t>28,12</t>
+        </is>
+      </c>
+    </row>
+    <row r="2936">
+      <c r="A2936" t="inlineStr">
+        <is>
+          <t>31.01.2025 13:45</t>
+        </is>
+      </c>
+      <c r="B2936" t="inlineStr">
+        <is>
+          <t>2,2</t>
+        </is>
+      </c>
+      <c r="C2936" t="inlineStr">
+        <is>
+          <t>28,52</t>
+        </is>
+      </c>
+    </row>
+    <row r="2937">
+      <c r="A2937" t="inlineStr">
+        <is>
+          <t>31.01.2025 14:00</t>
+        </is>
+      </c>
+      <c r="B2937" t="inlineStr">
+        <is>
+          <t>33,36</t>
+        </is>
+      </c>
+      <c r="C2937" t="inlineStr">
+        <is>
+          <t>4,88</t>
+        </is>
+      </c>
+    </row>
+    <row r="2938">
+      <c r="A2938" t="inlineStr">
+        <is>
+          <t>31.01.2025 14:15</t>
+        </is>
+      </c>
+      <c r="B2938" t="inlineStr">
+        <is>
+          <t>14,12</t>
+        </is>
+      </c>
+      <c r="C2938" t="inlineStr">
+        <is>
+          <t>29,96</t>
+        </is>
+      </c>
+    </row>
+    <row r="2939">
+      <c r="A2939" t="inlineStr">
+        <is>
+          <t>31.01.2025 14:30</t>
+        </is>
+      </c>
+      <c r="B2939" t="inlineStr">
+        <is>
+          <t>2,72</t>
+        </is>
+      </c>
+      <c r="C2939" t="inlineStr">
+        <is>
+          <t>35,92</t>
+        </is>
+      </c>
+    </row>
+    <row r="2940">
+      <c r="A2940" t="inlineStr">
+        <is>
+          <t>31.01.2025 14:45</t>
+        </is>
+      </c>
+      <c r="B2940" t="inlineStr">
+        <is>
+          <t>11,52</t>
+        </is>
+      </c>
+      <c r="C2940" t="inlineStr">
+        <is>
+          <t>55,24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2941">
+      <c r="A2941" t="inlineStr">
+        <is>
+          <t>31.01.2025 15:00</t>
+        </is>
+      </c>
+      <c r="B2941" t="inlineStr">
+        <is>
+          <t>6,68</t>
+        </is>
+      </c>
+      <c r="C2941" t="inlineStr">
+        <is>
+          <t>42,48</t>
+        </is>
+      </c>
+    </row>
+    <row r="2942">
+      <c r="A2942" t="inlineStr">
+        <is>
+          <t>31.01.2025 15:15</t>
+        </is>
+      </c>
+      <c r="B2942" t="inlineStr">
+        <is>
+          <t>3,96</t>
+        </is>
+      </c>
+      <c r="C2942" t="inlineStr">
+        <is>
+          <t>32,72</t>
+        </is>
+      </c>
+    </row>
+    <row r="2943">
+      <c r="A2943" t="inlineStr">
+        <is>
+          <t>31.01.2025 15:30</t>
+        </is>
+      </c>
+      <c r="B2943" t="inlineStr">
+        <is>
+          <t>0,84</t>
+        </is>
+      </c>
+      <c r="C2943" t="inlineStr">
+        <is>
+          <t>67,84</t>
+        </is>
+      </c>
+    </row>
+    <row r="2944">
+      <c r="A2944" t="inlineStr">
+        <is>
+          <t>31.01.2025 15:45</t>
+        </is>
+      </c>
+      <c r="B2944" t="inlineStr">
+        <is>
+          <t>124,16</t>
+        </is>
+      </c>
+      <c r="C2944" t="inlineStr">
+        <is>
+          <t>0,16</t>
+        </is>
+      </c>
+    </row>
+    <row r="2945">
+      <c r="A2945" t="inlineStr">
+        <is>
+          <t>31.01.2025 16:00</t>
+        </is>
+      </c>
+      <c r="B2945" t="inlineStr">
+        <is>
+          <t>3,2</t>
+        </is>
+      </c>
+      <c r="C2945" t="inlineStr">
+        <is>
+          <t>48,6</t>
+        </is>
+      </c>
+    </row>
+    <row r="2946">
+      <c r="A2946" t="inlineStr">
+        <is>
+          <t>31.01.2025 16:15</t>
+        </is>
+      </c>
+      <c r="B2946" t="inlineStr">
+        <is>
+          <t>33,68</t>
+        </is>
+      </c>
+      <c r="C2946" t="inlineStr">
+        <is>
+          <t>14,16</t>
+        </is>
+      </c>
+    </row>
+    <row r="2947">
+      <c r="A2947" t="inlineStr">
+        <is>
+          <t>31.01.2025 16:30</t>
+        </is>
+      </c>
+      <c r="B2947" t="inlineStr">
+        <is>
+          <t>5,56</t>
+        </is>
+      </c>
+      <c r="C2947" t="inlineStr">
+        <is>
+          <t>56,32</t>
+        </is>
+      </c>
+    </row>
+    <row r="2948">
+      <c r="A2948" t="inlineStr">
+        <is>
+          <t>31.01.2025 16:45</t>
+        </is>
+      </c>
+      <c r="B2948" t="inlineStr">
+        <is>
+          <t>162,2</t>
+        </is>
+      </c>
+      <c r="C2948" t="inlineStr">
+        <is>
+          <t>0,08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2949">
+      <c r="A2949" t="inlineStr">
+        <is>
+          <t>31.01.2025 17:00</t>
+        </is>
+      </c>
+      <c r="B2949" t="inlineStr">
+        <is>
+          <t>9,32</t>
+        </is>
+      </c>
+      <c r="C2949" t="inlineStr">
+        <is>
+          <t>31,48</t>
+        </is>
+      </c>
+    </row>
+    <row r="2950">
+      <c r="A2950" t="inlineStr">
+        <is>
+          <t>31.01.2025 17:15</t>
+        </is>
+      </c>
+      <c r="B2950" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C2950" t="inlineStr">
+        <is>
+          <t>24,88</t>
+        </is>
+      </c>
+    </row>
+    <row r="2951">
+      <c r="A2951" t="inlineStr">
+        <is>
+          <t>31.01.2025 17:30</t>
+        </is>
+      </c>
+      <c r="B2951" t="inlineStr">
+        <is>
+          <t>2,12</t>
+        </is>
+      </c>
+      <c r="C2951" t="inlineStr">
+        <is>
+          <t>89,4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2952">
+      <c r="A2952" t="inlineStr">
+        <is>
+          <t>31.01.2025 17:45</t>
+        </is>
+      </c>
+      <c r="B2952" t="inlineStr">
+        <is>
+          <t>0,04</t>
+        </is>
+      </c>
+      <c r="C2952" t="inlineStr">
+        <is>
+          <t>69,92</t>
+        </is>
+      </c>
+    </row>
+    <row r="2953">
+      <c r="A2953" t="inlineStr">
+        <is>
+          <t>31.01.2025 18:00</t>
+        </is>
+      </c>
+      <c r="B2953" t="inlineStr">
+        <is>
+          <t>1,44</t>
+        </is>
+      </c>
+      <c r="C2953" t="inlineStr">
+        <is>
+          <t>29,56</t>
+        </is>
+      </c>
+    </row>
+    <row r="2954">
+      <c r="A2954" t="inlineStr">
+        <is>
+          <t>31.01.2025 18:15</t>
+        </is>
+      </c>
+      <c r="B2954" t="inlineStr">
+        <is>
+          <t>181,84</t>
+        </is>
+      </c>
+      <c r="C2954" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2955">
+      <c r="A2955" t="inlineStr">
+        <is>
+          <t>31.01.2025 18:30</t>
+        </is>
+      </c>
+      <c r="B2955" t="inlineStr">
+        <is>
+          <t>7,64</t>
+        </is>
+      </c>
+      <c r="C2955" t="inlineStr">
+        <is>
+          <t>18,56</t>
+        </is>
+      </c>
+    </row>
+    <row r="2956">
+      <c r="A2956" t="inlineStr">
+        <is>
+          <t>31.01.2025 18:45</t>
+        </is>
+      </c>
+      <c r="B2956" t="inlineStr">
+        <is>
+          <t>182,44</t>
+        </is>
+      </c>
+      <c r="C2956" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2957">
+      <c r="A2957" t="inlineStr">
+        <is>
+          <t>31.01.2025 19:00</t>
+        </is>
+      </c>
+      <c r="B2957" t="inlineStr">
+        <is>
+          <t>8,36</t>
+        </is>
+      </c>
+      <c r="C2957" t="inlineStr">
+        <is>
+          <t>20,28</t>
+        </is>
+      </c>
+    </row>
+    <row r="2958">
+      <c r="A2958" t="inlineStr">
+        <is>
+          <t>31.01.2025 19:15</t>
+        </is>
+      </c>
+      <c r="B2958" t="inlineStr">
+        <is>
+          <t>0,08</t>
+        </is>
+      </c>
+      <c r="C2958" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+    </row>
+    <row r="2959">
+      <c r="A2959" t="inlineStr">
+        <is>
+          <t>31.01.2025 19:30</t>
+        </is>
+      </c>
+      <c r="B2959" t="inlineStr">
+        <is>
+          <t>4,72</t>
+        </is>
+      </c>
+      <c r="C2959" t="inlineStr">
+        <is>
+          <t>27,92</t>
+        </is>
+      </c>
+    </row>
+    <row r="2960">
+      <c r="A2960" t="inlineStr">
+        <is>
+          <t>31.01.2025 19:45</t>
+        </is>
+      </c>
+      <c r="B2960" t="inlineStr">
+        <is>
+          <t>8,32</t>
+        </is>
+      </c>
+      <c r="C2960" t="inlineStr">
+        <is>
+          <t>27,96</t>
+        </is>
+      </c>
+    </row>
+    <row r="2961">
+      <c r="A2961" t="inlineStr">
+        <is>
+          <t>31.01.2025 20:00</t>
+        </is>
+      </c>
+      <c r="B2961" t="inlineStr">
+        <is>
+          <t>2,36</t>
+        </is>
+      </c>
+      <c r="C2961" t="inlineStr">
+        <is>
+          <t>33,28</t>
+        </is>
+      </c>
+    </row>
+    <row r="2962">
+      <c r="A2962" t="inlineStr">
+        <is>
+          <t>31.01.2025 20:15</t>
+        </is>
+      </c>
+      <c r="B2962" t="inlineStr">
+        <is>
+          <t>2,52</t>
+        </is>
+      </c>
+      <c r="C2962" t="inlineStr">
+        <is>
+          <t>22,08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2963">
+      <c r="A2963" t="inlineStr">
+        <is>
+          <t>31.01.2025 20:30</t>
+        </is>
+      </c>
+      <c r="B2963" t="inlineStr">
+        <is>
+          <t>8,24</t>
+        </is>
+      </c>
+      <c r="C2963" t="inlineStr">
+        <is>
+          <t>46,2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2964">
+      <c r="A2964" t="inlineStr">
+        <is>
+          <t>31.01.2025 20:45</t>
+        </is>
+      </c>
+      <c r="B2964" t="inlineStr">
+        <is>
+          <t>157,56</t>
+        </is>
+      </c>
+      <c r="C2964" t="inlineStr">
+        <is>
+          <t>0,24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2965">
+      <c r="A2965" t="inlineStr">
+        <is>
+          <t>31.01.2025 21:00</t>
+        </is>
+      </c>
+      <c r="B2965" t="inlineStr">
+        <is>
+          <t>10,64</t>
+        </is>
+      </c>
+      <c r="C2965" t="inlineStr">
+        <is>
+          <t>15,08</t>
+        </is>
+      </c>
+    </row>
+    <row r="2966">
+      <c r="A2966" t="inlineStr">
+        <is>
+          <t>31.01.2025 21:15</t>
+        </is>
+      </c>
+      <c r="B2966" t="inlineStr">
+        <is>
+          <t>0,24</t>
+        </is>
+      </c>
+      <c r="C2966" t="inlineStr">
+        <is>
+          <t>42,48</t>
+        </is>
+      </c>
+    </row>
+    <row r="2967">
+      <c r="A2967" t="inlineStr">
+        <is>
+          <t>31.01.2025 21:30</t>
+        </is>
+      </c>
+      <c r="B2967" t="inlineStr">
+        <is>
+          <t>12,04</t>
+        </is>
+      </c>
+      <c r="C2967" t="inlineStr">
+        <is>
+          <t>36,44</t>
+        </is>
+      </c>
+    </row>
+    <row r="2968">
+      <c r="A2968" t="inlineStr">
+        <is>
+          <t>31.01.2025 21:45</t>
+        </is>
+      </c>
+      <c r="B2968" t="inlineStr">
+        <is>
+          <t>6,48</t>
+        </is>
+      </c>
+      <c r="C2968" t="inlineStr">
+        <is>
+          <t>10,84</t>
+        </is>
+      </c>
+    </row>
+    <row r="2969">
+      <c r="A2969" t="inlineStr">
+        <is>
+          <t>31.01.2025 22:00</t>
+        </is>
+      </c>
+      <c r="B2969" t="inlineStr">
+        <is>
+          <t>18,6</t>
+        </is>
+      </c>
+      <c r="C2969" t="inlineStr">
+        <is>
+          <t>10,28</t>
+        </is>
+      </c>
+    </row>
+    <row r="2970">
+      <c r="A2970" t="inlineStr">
+        <is>
+          <t>31.01.2025 22:15</t>
+        </is>
+      </c>
+      <c r="B2970" t="inlineStr">
+        <is>
+          <t>118,36</t>
+        </is>
+      </c>
+      <c r="C2970" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2971">
+      <c r="A2971" t="inlineStr">
+        <is>
+          <t>31.01.2025 22:30</t>
+        </is>
+      </c>
+      <c r="B2971" t="inlineStr">
+        <is>
+          <t>3,68</t>
+        </is>
+      </c>
+      <c r="C2971" t="inlineStr">
+        <is>
+          <t>51,24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2972">
+      <c r="A2972" t="inlineStr">
+        <is>
+          <t>31.01.2025 22:45</t>
+        </is>
+      </c>
+      <c r="B2972" t="inlineStr">
+        <is>
+          <t>0,08</t>
+        </is>
+      </c>
+      <c r="C2972" t="inlineStr">
+        <is>
+          <t>62,48</t>
+        </is>
+      </c>
+    </row>
+    <row r="2973">
+      <c r="A2973" t="inlineStr">
+        <is>
+          <t>31.01.2025 23:00</t>
+        </is>
+      </c>
+      <c r="B2973" t="inlineStr">
+        <is>
+          <t>7,96</t>
+        </is>
+      </c>
+      <c r="C2973" t="inlineStr">
+        <is>
+          <t>14,2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2974">
+      <c r="A2974" t="inlineStr">
+        <is>
+          <t>31.01.2025 23:15</t>
+        </is>
+      </c>
+      <c r="B2974" t="inlineStr">
+        <is>
+          <t>0,4</t>
+        </is>
+      </c>
+      <c r="C2974" t="inlineStr">
+        <is>
+          <t>105,96</t>
+        </is>
+      </c>
+    </row>
+    <row r="2975">
+      <c r="A2975" t="inlineStr">
+        <is>
+          <t>31.01.2025 23:30</t>
+        </is>
+      </c>
+      <c r="B2975" t="inlineStr">
+        <is>
+          <t>183,08</t>
+        </is>
+      </c>
+      <c r="C2975" t="inlineStr">
+        <is>
+          <t>0,12</t>
+        </is>
+      </c>
+    </row>
+    <row r="2976">
+      <c r="A2976" t="inlineStr">
+        <is>
+          <t>31.01.2025 23:45</t>
+        </is>
+      </c>
+      <c r="B2976" t="inlineStr">
+        <is>
+          <t>7,36</t>
+        </is>
+      </c>
+      <c r="C2976" t="inlineStr">
+        <is>
+          <t>34,72</t>
+        </is>
+      </c>
+    </row>
+    <row r="2977">
+      <c r="A2977" t="inlineStr">
+        <is>
+          <t>01.02.2025 00:00</t>
+        </is>
+      </c>
+      <c r="B2977" t="inlineStr">
+        <is>
+          <t>20,04</t>
+        </is>
+      </c>
+      <c r="C2977" t="inlineStr">
+        <is>
+          <t>23,16</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>